<commit_message>
Adding results page - PART 3
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mega\MO-DM\SITE\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0989A9C-B482-4865-8D98-4B8EB7D6BDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64486F66-F26B-441E-AC92-775F2024329E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{8F00384F-4ECD-42F1-A9C5-F3B3221CE6BF}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{8F00384F-4ECD-42F1-A9C5-F3B3221CE6BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="EVC" sheetId="1" r:id="rId1"/>
+    <sheet name="ESTRELAS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>OPÇÃO</t>
   </si>
@@ -52,6 +53,12 @@
   </si>
   <si>
     <t>EVC  - (0 A 1)</t>
+  </si>
+  <si>
+    <t>PONTUAÇÃO - ESTRELAS</t>
+  </si>
+  <si>
+    <t>PESO (0 - 1)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4067EC-F25C-404C-9BE4-92DA00893D63}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -604,4 +611,85 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79A321A-4CD5-4EF1-B13F-EF63A20C0660}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.05" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>(A2-1)/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B7" si="0">(A3-1)/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding results page - PART 5
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mega\MO-DM\SITE\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64486F66-F26B-441E-AC92-775F2024329E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EE204-82F2-4182-89E0-5BB0FE04A69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{8F00384F-4ECD-42F1-A9C5-F3B3221CE6BF}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{8F00384F-4ECD-42F1-A9C5-F3B3221CE6BF}"/>
   </bookViews>
   <sheets>
     <sheet name="EVC" sheetId="1" r:id="rId1"/>
-    <sheet name="ESTRELAS" sheetId="2" r:id="rId2"/>
+    <sheet name="STARS WEIGHT - V" sheetId="2" r:id="rId2"/>
+    <sheet name="AGREEMENT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>OPÇÃO</t>
   </si>
@@ -59,13 +60,114 @@
   </si>
   <si>
     <t>PESO (0 - 1)</t>
+  </si>
+  <si>
+    <t>LEGENDA</t>
+  </si>
+  <si>
+    <t>EVC | E | V</t>
+  </si>
+  <si>
+    <t>BAIXO</t>
+  </si>
+  <si>
+    <t>0,00 &lt;= X &lt; 0,40</t>
+  </si>
+  <si>
+    <t>MÉDIO</t>
+  </si>
+  <si>
+    <t>0,40 &lt;= X &lt; 0,70</t>
+  </si>
+  <si>
+    <t>ALTO</t>
+  </si>
+  <si>
+    <t>0,70 &lt;= X &lt;= 1,00</t>
+  </si>
+  <si>
+    <t>CUSTO</t>
+  </si>
+  <si>
+    <t>0,60 &lt;= X &lt;= 1,00</t>
+  </si>
+  <si>
+    <t>0,30 &lt;= X &lt; 0,60</t>
+  </si>
+  <si>
+    <t>0,00 &lt;= X &lt; 0,30</t>
+  </si>
+  <si>
+    <t>DECISION 1</t>
+  </si>
+  <si>
+    <t>DECISION 2</t>
+  </si>
+  <si>
+    <t>DECISION 3</t>
+  </si>
+  <si>
+    <t>JUDGE 1</t>
+  </si>
+  <si>
+    <t>JUDGE 2</t>
+  </si>
+  <si>
+    <t>VARIANCE</t>
+  </si>
+  <si>
+    <t>MVAR (MEAN VARIANCE)</t>
+  </si>
+  <si>
+    <t>AGREEMENT</t>
+  </si>
+  <si>
+    <t>DENOMINATOR</t>
+  </si>
+  <si>
+    <r>
+      <t>LOWER VALUE - LIKERT - X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>UPPER VALUE - LIKERT - X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/articles/10.3389/fpsyg.2017.00777/full</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,16 +191,107 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,11 +299,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -123,9 +332,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -138,6 +357,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>250166</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596357</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>97449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65E0551-9DB5-4A6A-8035-4A8266D01C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3252158" y="2156603"/>
+          <a:ext cx="4728410" cy="658167"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>232912</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>97948</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>71302</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFD0DB7E-FB51-B7EF-F036-CCEE8AF0BD7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3234904" y="2924355"/>
+          <a:ext cx="3005052" cy="588886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>258793</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>138022</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>509936</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>61496</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433B7939-B90C-8D61-3667-FD20C75D9EF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3260785" y="1406105"/>
+          <a:ext cx="251143" cy="285783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4067EC-F25C-404C-9BE4-92DA00893D63}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -450,9 +806,11 @@
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="27.25" customWidth="1"/>
     <col min="7" max="7" width="32.125" customWidth="1"/>
+    <col min="9" max="9" width="15.125" customWidth="1"/>
+    <col min="10" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="25.85" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,8 +832,12 @@
       <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -500,8 +862,12 @@
         <f>((B2*0.3+C2*0.3-D2*0.4)+1.8)/5</f>
         <v>0.26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -526,8 +892,14 @@
         <f t="shared" ref="G3:G6" si="2">((B3*0.3+C3*0.3-D3*0.4)+1.8)/5</f>
         <v>0.41999999999999993</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -552,8 +924,14 @@
         <f t="shared" si="2"/>
         <v>0.67999999999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -578,8 +956,14 @@
         <f t="shared" si="2"/>
         <v>-4.4408920985006264E-17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -604,9 +988,35 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
+      <c r="I7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
+      <c r="I8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="21.1" x14ac:dyDescent="0.35">
+      <c r="I9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -617,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79A321A-4CD5-4EF1-B13F-EF63A20C0660}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -692,4 +1102,143 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147BD823-4480-403A-A748-3957EE964A48}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4">
+        <f>_xlfn.VAR.P(B2:B3)</f>
+        <v>6.25</v>
+      </c>
+      <c r="C5" s="4">
+        <f>_xlfn.VAR.P(C2:C3)</f>
+        <v>6.25</v>
+      </c>
+      <c r="D5" s="4">
+        <f>_xlfn.VAR.P(D2:D3)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4">
+        <f>AVERAGE(B5:D5)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4">
+        <f>0.5*(B14^2+B13^2)-(0.5*(B14+B13))^2</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="14">
+        <f>1-(B9/B15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding results page - PART 6
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mega\MO-DM\SITE\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EE204-82F2-4182-89E0-5BB0FE04A69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B9578B-2525-4E22-BD57-398CEF3F37FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{8F00384F-4ECD-42F1-A9C5-F3B3221CE6BF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>OPÇÃO</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>0,00 &lt;= X &lt; 0,30</t>
-  </si>
-  <si>
-    <t>DECISION 1</t>
-  </si>
-  <si>
-    <t>DECISION 2</t>
-  </si>
-  <si>
-    <t>DECISION 3</t>
   </si>
   <si>
     <t>JUDGE 1</t>
@@ -319,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -341,6 +332,12 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,7 +793,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1025,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1106,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1121,64 +1118,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>25</v>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>6</v>
       </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="4">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16">
         <f>_xlfn.VAR.P(B2:B3)</f>
         <v>6.25</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="16">
         <f>_xlfn.VAR.P(C2:C3)</f>
         <v>6.25</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="16">
         <f>_xlfn.VAR.P(D2:D3)</f>
         <v>6.25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4">
         <f>AVERAGE(B5:D5)</f>
@@ -1187,7 +1189,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1195,7 +1197,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -1203,7 +1205,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4">
         <f>0.5*(B14^2+B13^2)-(0.5*(B14+B13))^2</f>
@@ -1224,7 +1226,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="14">
         <f>1-(B9/B15)</f>
@@ -1233,7 +1235,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>